<commit_message>
Ficha Estacion | Ficha Portatil
</commit_message>
<xml_diff>
--- a/Scripts_R210_FuerzaVenta/LIQ19_R110_30.b_CI_Ficha_Portatil_20190131_JAR.XLSX
+++ b/Scripts_R210_FuerzaVenta/LIQ19_R110_30.b_CI_Ficha_Portatil_20190131_JAR.XLSX
@@ -5,19 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2019.Proyectos\LIQ19_Liquidaciones\LIQ19_SQL\Scripts_R110_Catalogos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tomza.TI\JArciniegaR.TI\1.SOL_Soluciones\LIQ19_Liquidaciones\Codigo\CodigoSQL\LIQ19_Liberacion_R0.00_Base_V0004\Scripts_R210_FuerzaVenta\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20438" windowHeight="7598"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20445" windowHeight="7605"/>
   </bookViews>
   <sheets>
     <sheet name="PRODUCTO" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PRODUCTO!$M$2:$M$53</definedName>
-  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="183">
   <si>
     <t>K_PUNTO_VENTA</t>
   </si>
@@ -363,27 +360,15 @@
     <t>MATRICULA</t>
   </si>
   <si>
-    <t>ABC123</t>
-  </si>
-  <si>
     <t>BCD345</t>
   </si>
   <si>
-    <t>EDE657</t>
-  </si>
-  <si>
     <t>FEFE889</t>
   </si>
   <si>
     <t>MAT123</t>
   </si>
   <si>
-    <t>MARCA</t>
-  </si>
-  <si>
-    <t>CHEVROLET</t>
-  </si>
-  <si>
     <t>MODELO</t>
   </si>
   <si>
@@ -408,9 +393,6 @@
     <t>DW31616</t>
   </si>
   <si>
-    <t>DX06774</t>
-  </si>
-  <si>
     <t>DV10363</t>
   </si>
   <si>
@@ -423,9 +405,6 @@
     <t>DV10456</t>
   </si>
   <si>
-    <t>DV10458</t>
-  </si>
-  <si>
     <t>DV10419</t>
   </si>
   <si>
@@ -435,12 +414,6 @@
     <t>DV10359</t>
   </si>
   <si>
-    <t>GMC</t>
-  </si>
-  <si>
-    <t>GENERAL MOTORSS</t>
-  </si>
-  <si>
     <t>2006</t>
   </si>
   <si>
@@ -465,15 +438,6 @@
     <t>61784</t>
   </si>
   <si>
-    <t>1996</t>
-  </si>
-  <si>
-    <t>170980</t>
-  </si>
-  <si>
-    <t>G.M.KODIAK</t>
-  </si>
-  <si>
     <t>2005</t>
   </si>
   <si>
@@ -495,27 +459,9 @@
     <t>2443861</t>
   </si>
   <si>
-    <t>1946859</t>
-  </si>
-  <si>
-    <t>1978555</t>
-  </si>
-  <si>
     <t>1276028</t>
   </si>
   <si>
-    <t>GMC C7500</t>
-  </si>
-  <si>
-    <t>2001</t>
-  </si>
-  <si>
-    <t>1733700</t>
-  </si>
-  <si>
-    <t>NISSAN</t>
-  </si>
-  <si>
     <t>2010</t>
   </si>
   <si>
@@ -525,15 +471,9 @@
     <t>17711</t>
   </si>
   <si>
-    <t>CHEVROLET HEAVY DUTY</t>
-  </si>
-  <si>
     <t>2007</t>
   </si>
   <si>
-    <t>1.9</t>
-  </si>
-  <si>
     <t>22098</t>
   </si>
   <si>
@@ -543,15 +483,9 @@
     <t>228.6</t>
   </si>
   <si>
-    <t>31741</t>
-  </si>
-  <si>
     <t>8911979</t>
   </si>
   <si>
-    <t>NISSAN VPM</t>
-  </si>
-  <si>
     <t>2008</t>
   </si>
   <si>
@@ -561,9 +495,6 @@
     <t>3GBKC34G55M118806</t>
   </si>
   <si>
-    <t>3GBKC34G75M118922</t>
-  </si>
-  <si>
     <t>1GDJ7H1E4J901664</t>
   </si>
   <si>
@@ -579,15 +510,9 @@
     <t>1GDG6H1P9RJ519414</t>
   </si>
   <si>
-    <t>3GCM7HIMXVM501317</t>
-  </si>
-  <si>
     <t>1GBM7H1P2PJ101461</t>
   </si>
   <si>
-    <t>1G1GDJ6H1BXXJ504086</t>
-  </si>
-  <si>
     <t>3GBJ6H1E45M105516</t>
   </si>
   <si>
@@ -600,27 +525,15 @@
     <t>3GBM7H1E62M104342</t>
   </si>
   <si>
-    <t>3GBM7H1E52M104266</t>
-  </si>
-  <si>
-    <t>1GBL7H1PXRJ1078</t>
-  </si>
-  <si>
     <t>1GDG6H1P6TJ504599</t>
   </si>
   <si>
-    <t>1GDJ7H1E12J505377</t>
-  </si>
-  <si>
     <t>013FB0473C4F544B</t>
   </si>
   <si>
     <t>0136B07390508612</t>
   </si>
   <si>
-    <t>3N6DD14577K040339</t>
-  </si>
-  <si>
     <t>013AB067801076420</t>
   </si>
   <si>
@@ -630,33 +543,21 @@
     <t>3N6DD14568K002327</t>
   </si>
   <si>
-    <t>0144S02470505EAB</t>
-  </si>
-  <si>
     <t>3NGDD14528K021599</t>
   </si>
   <si>
     <t>5000</t>
   </si>
   <si>
-    <t>12200</t>
-  </si>
-  <si>
     <t>12500</t>
   </si>
   <si>
-    <t>10000</t>
-  </si>
-  <si>
     <t>8250</t>
   </si>
   <si>
     <t>8670</t>
   </si>
   <si>
-    <t>10500</t>
-  </si>
-  <si>
     <t>6850</t>
   </si>
   <si>
@@ -669,10 +570,10 @@
     <t>1866</t>
   </si>
   <si>
-    <t>tipo</t>
-  </si>
-  <si>
     <t>K_DETALLE_PORTATIL</t>
+  </si>
+  <si>
+    <t>K_MARCA</t>
   </si>
 </sst>
 </file>
@@ -1048,1732 +949,1054 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="B2:R53"/>
+  <dimension ref="B2:Q35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J4" sqref="J4:J53"/>
+      <selection pane="bottomRight" activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.19921875" customWidth="1"/>
-    <col min="2" max="2" width="13.1328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.06640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.796875" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.06640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" style="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="122.1328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.53125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.53125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="31.86328125" customWidth="1"/>
-    <col min="16" max="16" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="122.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="31.85546875" customWidth="1"/>
+    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" s="4" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
-        <v>214</v>
+        <v>181</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="F2" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>120</v>
-      </c>
       <c r="I2" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="R2" s="2"/>
-    </row>
-    <row r="3" spans="2:18" hidden="1" x14ac:dyDescent="0.45">
+        <v>117</v>
+      </c>
+      <c r="Q2" s="2"/>
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3" s="3">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="12">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>111</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>122</v>
+      <c r="F3" s="12">
+        <v>2006</v>
       </c>
       <c r="G3" s="12">
-        <v>0</v>
+        <v>233859</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>122</v>
+        <v>155</v>
       </c>
       <c r="I3" s="14">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2" t="e">
-        <f>CONCATENATE("EXECUTE [dbo].[PG_CI_DETALLE_AUTOTANQUE] 0,0, ",B3,", ",C3,", ",#REF!,",",#REF!,",'",D3,"','",E3,"','",F3,"',",G3,",'",H3,"',",I3,",'",#REF!,"','",#REF!,"','",#REF!,"'; ")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M3" s="8">
-        <v>1</v>
-      </c>
-      <c r="N3" s="1"/>
-      <c r="R3" s="2"/>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.45">
+        <v>5000</v>
+      </c>
+      <c r="J3" s="2" t="str">
+        <f>CONCATENATE("EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, ",B3,", ",C3,",",D3,",'",E3,"','",F3,"',",G3,",'",H3,"',",I3,"; ")</f>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 1, 2,1,'BCD345','2006',233859,'3GBKC34G55M118806',5000; </v>
+      </c>
+      <c r="N3" s="6"/>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="12">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
         <v>112</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>117</v>
-      </c>
       <c r="F4" s="12">
-        <v>2006</v>
+        <v>2002</v>
       </c>
       <c r="G4" s="12">
-        <v>233859</v>
+        <v>1522039</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="I4" s="14">
-        <v>5000</v>
+        <v>11315</v>
       </c>
       <c r="J4" s="2" t="str">
-        <f>CONCATENATE("EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, ",B4,", ",C4,",'",D4,"','",E4,"','",F4,"',",G4,",'",H4,"',",I4,"; ")</f>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, 1, 2,'BCD345','CHEVROLET','2006',233859,'3GBKC34G55M118806',5000; </v>
-      </c>
-      <c r="M4" s="8">
-        <v>3</v>
-      </c>
-      <c r="O4" s="6"/>
-    </row>
-    <row r="5" spans="2:18" hidden="1" x14ac:dyDescent="0.45">
+        <f t="shared" ref="J4:J35" si="0">CONCATENATE("EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, ",B4,", ",C4,",",D4,",'",E4,"','",F4,"',",G4,",'",H4,"',",I4,"; ")</f>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 2, 4,2,'FEFE889','2002',1522039,'1GDJ7H1E4J901664',11315; </v>
+      </c>
+      <c r="N4" s="7"/>
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>3</v>
       </c>
       <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="12">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
         <v>113</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>117</v>
-      </c>
       <c r="F5" s="12">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="G5" s="12">
-        <v>861705</v>
+        <v>0</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="I5" s="14">
         <v>5000</v>
       </c>
-      <c r="J5" s="2" t="e">
-        <f>CONCATENATE("EXECUTE [dbo].[PG_CI_DETALLE_PUNTO_VENTA] 0,0, ",B5,", ",C5,", ",#REF!,",",#REF!,",'",D5,"','",E5,"','",F5,"',",G5,",'",H5,"',",I5,",'",#REF!,"','",#REF!,"','",#REF!,"'; ")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M5" s="8">
-        <v>2</v>
-      </c>
-      <c r="O5" s="7"/>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.45">
+      <c r="J5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 3, 5,3,'MAT123','2005',0,'3GBKC34GX5M101984',5000; </v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C6">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>114</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="F6" s="12">
-        <v>2002</v>
-      </c>
-      <c r="G6" s="12">
-        <v>1522039</v>
+        <v>6</v>
+      </c>
+      <c r="D6" s="12">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>130</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="I6" s="14">
-        <v>11315</v>
+        <v>4300</v>
       </c>
       <c r="J6" s="2" t="str">
-        <f t="shared" ref="J6:J9" si="0">CONCATENATE("EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, ",B6,", ",C6,",'",D6,"','",E6,"','",F6,"',",G6,",'",H6,"',",I6,"; ")</f>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, 2, 4,'FEFE889','GMC','2002',1522039,'1GDJ7H1E4J901664',11315; </v>
-      </c>
-      <c r="M6" s="8">
-        <v>3</v>
-      </c>
-      <c r="O6" s="7"/>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 4, 6,4,'N/D','2006',164292,'3GBKC34G55M118837',4300; </v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7" s="12">
         <v>5</v>
       </c>
-      <c r="D7" t="s">
-        <v>115</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="F7" s="12">
-        <v>2005</v>
-      </c>
-      <c r="G7" s="12">
-        <v>0</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="I7" s="14">
-        <v>5000</v>
+      <c r="E7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>173</v>
       </c>
       <c r="J7" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, 3, 5,'MAT123','GENERAL MOTORSS','2005',0,'3GBKC34GX5M101984',5000; </v>
-      </c>
-      <c r="M7" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.45">
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 5, 7,5,'DV10365','2006',141076,'3GBKC34GX5M118915',5000; </v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C8">
+        <v>9</v>
+      </c>
+      <c r="D8" s="12">
         <v>6</v>
       </c>
-      <c r="D8" t="s">
-        <v>122</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>117</v>
+      <c r="E8" s="15" t="s">
+        <v>120</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="I8" s="14">
-        <v>4300</v>
+        <v>134</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>174</v>
       </c>
       <c r="J8" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, 4, 6,'N/D','CHEVROLET','2006',164292,'3GBKC34G55M118837',4300; </v>
-      </c>
-      <c r="M8" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.45">
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 6, 9,6,'ZTV6503','1997',1578795,'1GDG6H1P9RJ519414',12500; </v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C9">
-        <v>7</v>
-      </c>
-      <c r="D9" t="s">
-        <v>123</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>117</v>
+        <v>10</v>
+      </c>
+      <c r="D9" s="12">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>121</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>181</v>
+        <v>118</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>202</v>
+        <v>174</v>
       </c>
       <c r="J9" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, 5, 7,'DV10365','CHEVROLET','2006',141076,'3GBKC34GX5M118915',5000; </v>
-      </c>
-      <c r="M9" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="2:18" hidden="1" x14ac:dyDescent="0.45">
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 7, 10,1,'DW31616','N/D',0,'N/D',12500; </v>
+      </c>
+      <c r="N9" s="15"/>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>8</v>
       </c>
       <c r="C10">
-        <v>8</v>
-      </c>
-      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="12">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
         <v>122</v>
       </c>
-      <c r="E10" s="12" t="s">
-        <v>122</v>
-      </c>
       <c r="F10" s="12" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="G10" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="J10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 8, 12,2,'DV10363','1990',61784,'1GBM7H1P2PJ101461',12500; </v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B11" s="3">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>14</v>
+      </c>
+      <c r="D11" s="12">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>118</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="J11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 9, 14,3,'N/D','2005',0,'3GBJ6H1E45M105516',8250; </v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B12" s="3">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>15</v>
+      </c>
+      <c r="D12" s="12">
+        <v>4</v>
+      </c>
+      <c r="E12" t="s">
+        <v>118</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="J12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 10, 15,4,'N/D','1995',2099804,'1G017H1P45J520018',12500; </v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B13" s="3">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>16</v>
+      </c>
+      <c r="D13" s="12">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>123</v>
+      </c>
+      <c r="F13" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="J10" s="2" t="e">
-        <f>CONCATENATE("EXECUTE [dbo].[PG_CI_DETALLE_PUNTO_VENTA] 0,0, ",B10,", ",C10,", ",#REF!,",",#REF!,",'",D10,"','",E10,"','",F10,"',",G10,",'",H10,"',",I10,",'",#REF!,"','",#REF!,"','",#REF!,"'; ")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M10" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B11" s="3">
+      <c r="G13" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="J13" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 11, 16,5,'DV10362','1992',1881350,'1GDG6H1T7PJ504326',8670; </v>
+      </c>
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B14" s="3">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>17</v>
+      </c>
+      <c r="D14" s="12">
         <v>6</v>
       </c>
-      <c r="C11">
-        <v>9</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="G11" s="12" t="s">
+      <c r="E14" t="s">
+        <v>118</v>
+      </c>
+      <c r="F14" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="J11" s="2" t="str">
-        <f t="shared" ref="J11:J12" si="1">CONCATENATE("EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, ",B11,", ",C11,",'",D11,"','",E11,"','",F11,"',",G11,",'",H11,"',",I11,"; ")</f>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, 6, 9,'ZTV6503','GMC','1997',1578795,'1GDG6H1P9RJ519414',12500; </v>
-      </c>
-      <c r="M11" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B12" s="3">
-        <v>7</v>
-      </c>
-      <c r="C12">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>125</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="J12" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, 7, 10,'DW31616','N/D','N/D',0,'N/D',12500; </v>
-      </c>
-      <c r="M12" s="8">
-        <v>3</v>
-      </c>
-      <c r="O12" s="15"/>
-    </row>
-    <row r="13" spans="2:18" hidden="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="3">
-        <v>2</v>
-      </c>
-      <c r="C13">
-        <v>11</v>
-      </c>
-      <c r="D13" t="s">
-        <v>126</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="I13" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="J13" s="2" t="e">
-        <f>CONCATENATE("EXECUTE [dbo].[PG_CI_DETALLE_AUTOTANQUE] 0,0, ",B13,", ",C13,", ",#REF!,",",#REF!,",'",D13,"','",E13,"','",F13,"',",G13,",'",H13,"',",I13,",'",#REF!,"','",#REF!,"','",#REF!,"'; ")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M13" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B14" s="3">
-        <v>8</v>
-      </c>
-      <c r="C14">
-        <v>12</v>
-      </c>
-      <c r="D14" t="s">
-        <v>127</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="F14" s="12" t="s">
+      <c r="G14" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="G14" s="12" t="s">
-        <v>144</v>
-      </c>
       <c r="H14" s="1" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
       <c r="I14" s="13" t="s">
-        <v>204</v>
+        <v>174</v>
       </c>
       <c r="J14" s="2" t="str">
-        <f>CONCATENATE("EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, ",B14,", ",C14,",'",D14,"','",E14,"','",F14,"',",G14,",'",H14,"',",I14,"; ")</f>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, 8, 12,'DV10363','GMC','1990',61784,'1GBM7H1P2PJ101461',12500; </v>
-      </c>
-      <c r="M14" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="2:18" hidden="1" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 12, 17,6,'N/D','2002',2443861,'3GBM7H1E62M104342',12500; </v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <v>13</v>
       </c>
       <c r="C15">
-        <v>13</v>
-      </c>
-      <c r="D15" t="s">
-        <v>122</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>135</v>
+        <v>19</v>
+      </c>
+      <c r="D15" s="12">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>124</v>
       </c>
       <c r="F15" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="J15" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 13, 19,1,'DY-2983','N/D',0,'N/D',12500; </v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B16" s="3">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>20</v>
+      </c>
+      <c r="D16" s="12">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>118</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="J16" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 14, 20,2,'N/D','N/D',0,'N/D',12500; </v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="3">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>22</v>
+      </c>
+      <c r="D17" s="12">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>125</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="J17" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 15, 22,3,'DV10456','1995',1276028,'1GDG6H1P6TJ504599',12500; </v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="3">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>24</v>
+      </c>
+      <c r="D18" s="12">
+        <v>4</v>
+      </c>
+      <c r="E18" t="s">
+        <v>118</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="J18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 16, 24,4,'N/D','N/D',0,'N/D',6850; </v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="3">
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <v>25</v>
+      </c>
+      <c r="D19" s="12">
+        <v>5</v>
+      </c>
+      <c r="E19" t="s">
+        <v>118</v>
+      </c>
+      <c r="F19" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="G15" s="12" t="s">
+      <c r="G19" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="I15" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="J15" s="2" t="e">
-        <f>CONCATENATE("EXECUTE [dbo].[PG_CI_DETALLE_PUNTO_VENTA] 0,0, ",B15,", ",C15,", ",#REF!,",",#REF!,",'",D15,"','",E15,"','",F15,"',",G15,",'",H15,"',",I15,",'",#REF!,"','",#REF!,"','",#REF!,"'; ")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M15" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.45">
-      <c r="B16" s="3">
-        <v>9</v>
-      </c>
-      <c r="C16">
-        <v>14</v>
-      </c>
-      <c r="D16" t="s">
-        <v>122</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="I16" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="J16" s="2" t="str">
-        <f t="shared" ref="J16:J19" si="2">CONCATENATE("EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, ",B16,", ",C16,",'",D16,"','",E16,"','",F16,"',",G16,",'",H16,"',",I16,"; ")</f>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, 9, 14,'N/D','G.M.KODIAK','2005',0,'3GBJ6H1E45M105516',8250; </v>
-      </c>
-      <c r="M16" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B17" s="3">
-        <v>10</v>
-      </c>
-      <c r="C17">
-        <v>15</v>
-      </c>
-      <c r="D17" t="s">
-        <v>122</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="I17" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="J17" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, 10, 15,'N/D','GMC','1995',2099804,'1G017H1P45J520018',12500; </v>
-      </c>
-      <c r="M17" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B18" s="3">
-        <v>11</v>
-      </c>
-      <c r="C18">
-        <v>16</v>
-      </c>
-      <c r="D18" t="s">
-        <v>128</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="I18" s="13" t="s">
-        <v>207</v>
-      </c>
-      <c r="J18" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, 11, 16,'DV10362','GMC','1992',1881350,'1GDG6H1T7PJ504326',8670; </v>
-      </c>
-      <c r="M18" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B19" s="3">
-        <v>12</v>
-      </c>
-      <c r="C19">
-        <v>17</v>
-      </c>
-      <c r="D19" t="s">
-        <v>122</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>154</v>
-      </c>
       <c r="H19" s="1" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>204</v>
+        <v>132</v>
       </c>
       <c r="J19" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, 12, 17,'N/D','CHEVROLET','2002',2443861,'3GBM7H1E62M104342',12500; </v>
-      </c>
-      <c r="M19" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13" hidden="1" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 17, 25,5,'N/D','2010',29056,'013FB0473C4F544B',0; </v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <v>18</v>
       </c>
       <c r="C20">
-        <v>18</v>
-      </c>
-      <c r="D20" t="s">
-        <v>122</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>117</v>
+        <v>26</v>
+      </c>
+      <c r="D20" s="12">
+        <v>6</v>
+      </c>
+      <c r="E20" t="s">
+        <v>118</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>190</v>
+        <v>168</v>
       </c>
       <c r="I20" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="J20" s="2" t="e">
-        <f>CONCATENATE("EXECUTE [dbo].[PG_CI_DETALLE_PUNTO_VENTA] 0,0, ",B20,", ",C20,", ",#REF!,",",#REF!,",'",D20,"','",E20,"','",F20,"',",G20,",'",H20,"',",I20,",'",#REF!,"','",#REF!,"','",#REF!,"'; ")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M20" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+      <c r="J20" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 18, 26,6,'N/D','2010',17711,'0136B07390508612',0; </v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C21">
-        <v>19</v>
-      </c>
-      <c r="D21" t="s">
-        <v>129</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>122</v>
+        <v>27</v>
+      </c>
+      <c r="D21" s="12">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>126</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I21" s="13" t="s">
-        <v>204</v>
+        <v>132</v>
       </c>
       <c r="J21" s="2" t="str">
-        <f t="shared" ref="J21:J22" si="3">CONCATENATE("EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, ",B21,", ",C21,",'",D21,"','",E21,"','",F21,"',",G21,",'",H21,"',",I21,"; ")</f>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, 13, 19,'DY-2983','N/D','N/D',0,'N/D',12500; </v>
-      </c>
-      <c r="M21" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 19, 27,1,'DV10419','N/D',0,'N/D',0; </v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C22">
-        <v>20</v>
-      </c>
-      <c r="D22" t="s">
-        <v>122</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>135</v>
+        <v>29</v>
+      </c>
+      <c r="D22" s="12">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>118</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>122</v>
+        <v>145</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>122</v>
+        <v>168</v>
       </c>
       <c r="I22" s="13" t="s">
-        <v>204</v>
+        <v>132</v>
       </c>
       <c r="J22" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, 14, 20,'N/D','GMC','N/D',0,'N/D',12500; </v>
-      </c>
-      <c r="M22" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="2:13" hidden="1" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 20, 29,2,'N/D','2010',0,'0136B07390508612',0; </v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C23">
-        <v>21</v>
-      </c>
-      <c r="D23" t="s">
-        <v>122</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>135</v>
+        <v>30</v>
+      </c>
+      <c r="D23" s="12">
+        <v>3</v>
+      </c>
+      <c r="E23" t="s">
+        <v>118</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="I23" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="J23" s="2" t="e">
-        <f>CONCATENATE("EXECUTE [dbo].[PG_CI_DETALLE_AUTOTANQUE] 0,0, ",B23,", ",C23,", ",#REF!,",",#REF!,",'",D23,"','",E23,"','",F23,"',",G23,",'",H23,"',",I23,",'",#REF!,"','",#REF!,"','",#REF!,"'; ")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M23" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+      <c r="J23" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 21, 30,3,'N/D','2010',22098,'013AB067801076420',0; </v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="3">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C24">
-        <v>22</v>
-      </c>
-      <c r="D24" t="s">
-        <v>130</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>135</v>
+        <v>32</v>
+      </c>
+      <c r="D24" s="12">
+        <v>4</v>
+      </c>
+      <c r="E24" t="s">
+        <v>118</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>149</v>
+        <v>118</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>157</v>
+        <v>132</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>192</v>
+        <v>118</v>
       </c>
       <c r="I24" s="13" t="s">
-        <v>204</v>
+        <v>132</v>
       </c>
       <c r="J24" s="2" t="str">
-        <f>CONCATENATE("EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, ",B24,", ",C24,",'",D24,"','",E24,"','",F24,"',",G24,",'",H24,"',",I24,"; ")</f>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, 15, 22,'DV10456','GMC','1995',1276028,'1GDG6H1P6TJ504599',12500; </v>
-      </c>
-      <c r="M24" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="2:13" hidden="1" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 22, 32,4,'N/D','N/D',0,'N/D',0; </v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <v>23</v>
       </c>
       <c r="C25">
-        <v>23</v>
-      </c>
-      <c r="D25" t="s">
-        <v>131</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>158</v>
+        <v>34</v>
+      </c>
+      <c r="D25" s="12">
+        <v>5</v>
+      </c>
+      <c r="E25" t="s">
+        <v>118</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>159</v>
+        <v>118</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>160</v>
+        <v>132</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>193</v>
+        <v>118</v>
       </c>
       <c r="I25" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="J25" s="2" t="e">
-        <f>CONCATENATE("EXECUTE [dbo].[PG_CI_DETALLE_PUNTO_VENTA] 0,0, ",B25,", ",C25,", ",#REF!,",",#REF!,",'",D25,"','",E25,"','",F25,"',",G25,",'",H25,"',",I25,",'",#REF!,"','",#REF!,"','",#REF!,"'; ")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M25" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+      <c r="J25" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 23, 34,5,'N/D','N/D',0,'N/D',0; </v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C26">
-        <v>24</v>
-      </c>
-      <c r="D26" t="s">
-        <v>122</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>135</v>
+        <v>35</v>
+      </c>
+      <c r="D26" s="12">
+        <v>6</v>
+      </c>
+      <c r="E26" t="s">
+        <v>118</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>122</v>
+        <v>148</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>122</v>
+        <v>170</v>
       </c>
       <c r="I26" s="13" t="s">
-        <v>209</v>
+        <v>132</v>
       </c>
       <c r="J26" s="2" t="str">
-        <f t="shared" ref="J26:J29" si="4">CONCATENATE("EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, ",B26,", ",C26,",'",D26,"','",E26,"','",F26,"',",G26,",'",H26,"',",I26,"; ")</f>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, 16, 24,'N/D','GMC','N/D',0,'N/D',6850; </v>
-      </c>
-      <c r="M26" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 24, 35,6,'N/D','2007',1.3,'3N6DD14547K040525',0; </v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C27">
-        <v>25</v>
-      </c>
-      <c r="D27" t="s">
-        <v>122</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>161</v>
+        <v>36</v>
+      </c>
+      <c r="D27" s="12">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>118</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>162</v>
+        <v>118</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>163</v>
+        <v>132</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>194</v>
+        <v>118</v>
       </c>
       <c r="I27" s="13" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="J27" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, 17, 25,'N/D','NISSAN','2010',29056,'013FB0473C4F544B',0; </v>
-      </c>
-      <c r="M27" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 25, 36,1,'N/D','N/D',0,'N/D',0; </v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C28">
-        <v>26</v>
-      </c>
-      <c r="D28" t="s">
-        <v>122</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>161</v>
+        <v>37</v>
+      </c>
+      <c r="D28" s="12">
+        <v>2</v>
+      </c>
+      <c r="E28" t="s">
+        <v>118</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>195</v>
+        <v>171</v>
       </c>
       <c r="I28" s="13" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="J28" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, 18, 26,'N/D','NISSAN','2010',17711,'0136B07390508612',0; </v>
-      </c>
-      <c r="M28" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 26, 37,2,'N/D','2007',228.6,'3N6DD14568K002327',0; </v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="3">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C29">
-        <v>27</v>
-      </c>
-      <c r="D29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="12">
+        <v>3</v>
+      </c>
+      <c r="E29" t="s">
+        <v>118</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="G29" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="E29" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>140</v>
-      </c>
       <c r="H29" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="J29" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, 19, 27,'DV10419','CHEVROLET HEAVY DUTY','N/D',0,'N/D',0; </v>
-      </c>
-      <c r="M29" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="2:13" hidden="1" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 27, 39,3,'N/D','N/D',0,'N/D',0; </v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <v>28</v>
       </c>
       <c r="C30">
-        <v>28</v>
-      </c>
-      <c r="D30" t="s">
-        <v>122</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>161</v>
+        <v>40</v>
+      </c>
+      <c r="D30" s="12">
+        <v>4</v>
+      </c>
+      <c r="E30" t="s">
+        <v>127</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>166</v>
+        <v>118</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>167</v>
+        <v>132</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>196</v>
+        <v>118</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="J30" s="2" t="e">
-        <f>CONCATENATE("EXECUTE [dbo].[PG_CI_DETALLE_PUNTO_VENTA] 0,0, ",B30,", ",C30,", ",#REF!,",",#REF!,",'",D30,"','",E30,"','",F30,"',",G30,",'",H30,"',",I30,",'",#REF!,"','",#REF!,"','",#REF!,"'; ")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M30" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.45">
+        <v>132</v>
+      </c>
+      <c r="J30" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 28, 40,4,'DV10353','N/D',0,'N/D',0; </v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="3">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C31">
-        <v>29</v>
-      </c>
-      <c r="D31" t="s">
-        <v>122</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>161</v>
+        <v>42</v>
+      </c>
+      <c r="D31" s="12">
+        <v>5</v>
+      </c>
+      <c r="E31" t="s">
+        <v>128</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>162</v>
+        <v>118</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>195</v>
+        <v>118</v>
       </c>
       <c r="I31" s="13" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="J31" s="2" t="str">
-        <f t="shared" ref="J31:J32" si="5">CONCATENATE("EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, ",B31,", ",C31,",'",D31,"','",E31,"','",F31,"',",G31,",'",H31,"',",I31,"; ")</f>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, 20, 29,'N/D','NISSAN','2010',0,'0136B07390508612',0; </v>
-      </c>
-      <c r="M31" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 29, 42,5,'DV10359','N/D',0,'N/D',0; </v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="3">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C32">
-        <v>30</v>
-      </c>
-      <c r="D32" t="s">
-        <v>122</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>161</v>
+        <v>44</v>
+      </c>
+      <c r="D32" s="12">
+        <v>6</v>
+      </c>
+      <c r="E32" t="s">
+        <v>118</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>162</v>
+        <v>118</v>
       </c>
       <c r="G32" s="12" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>197</v>
+        <v>118</v>
       </c>
       <c r="I32" s="13" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="J32" s="2" t="str">
-        <f t="shared" si="5"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, 21, 30,'N/D','NISSAN','2010',22098,'013AB067801076420',0; </v>
-      </c>
-      <c r="M32" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="2:13" hidden="1" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 30, 44,6,'N/D','N/D',8911979,'N/D',0; </v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="3">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C33">
-        <v>31</v>
-      </c>
-      <c r="D33" t="s">
-        <v>122</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>122</v>
+        <v>45</v>
+      </c>
+      <c r="D33" s="12">
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
+        <v>118</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="G33" s="12" t="s">
-        <v>140</v>
+        <v>118</v>
+      </c>
+      <c r="G33" s="12">
+        <v>0</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I33" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="J33" s="2" t="e">
-        <f>CONCATENATE("EXECUTE [dbo].[PG_CI_DETALLE_AUTOTANQUE] 0,0, ",B33,", ",C33,", ",#REF!,",",#REF!,",'",D33,"','",E33,"','",F33,"',",G33,",'",H33,"',",I33,",'",#REF!,"','",#REF!,"','",#REF!,"'; ")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M33" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.45">
+        <v>178</v>
+      </c>
+      <c r="J33" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 31, 45,1,'N/D','N/D',0,'N/D',4750; </v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="3">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C34">
-        <v>32</v>
-      </c>
-      <c r="D34" t="s">
-        <v>122</v>
-      </c>
-      <c r="E34" s="12" t="s">
-        <v>122</v>
+        <v>46</v>
+      </c>
+      <c r="D34" s="12">
+        <v>2</v>
+      </c>
+      <c r="E34" t="s">
+        <v>118</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="G34" s="12" t="s">
-        <v>140</v>
+        <v>118</v>
+      </c>
+      <c r="G34" s="12">
+        <v>0</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="I34" s="13" t="s">
-        <v>140</v>
+        <v>179</v>
       </c>
       <c r="J34" s="2" t="str">
-        <f>CONCATENATE("EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, ",B34,", ",C34,",'",D34,"','",E34,"','",F34,"',",G34,",'",H34,"',",I34,"; ")</f>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, 22, 32,'N/D','N/D','N/D',0,'N/D',0; </v>
-      </c>
-      <c r="M34" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="2:13" hidden="1" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 32, 46,2,'N/D','N/D',0,'N/D',3500; </v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="3">
         <v>33</v>
       </c>
       <c r="C35">
-        <v>33</v>
-      </c>
-      <c r="D35" t="s">
-        <v>133</v>
-      </c>
-      <c r="E35" s="12" t="s">
-        <v>122</v>
+        <v>47</v>
+      </c>
+      <c r="D35" s="12">
+        <v>3</v>
+      </c>
+      <c r="E35" t="s">
+        <v>118</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>122</v>
+        <v>153</v>
       </c>
       <c r="G35" s="12" t="s">
-        <v>140</v>
+        <v>154</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>122</v>
+        <v>172</v>
       </c>
       <c r="I35" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="J35" s="2" t="e">
-        <f>CONCATENATE("EXECUTE [dbo].[PG_CI_DETALLE_PUNTO_VENTA] 0,0, ",B35,", ",C35,", ",#REF!,",",#REF!,",'",D35,"','",E35,"','",F35,"',",G35,",'",H35,"',",I35,",'",#REF!,"','",#REF!,"','",#REF!,"'; ")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M35" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B36" s="3">
-        <v>23</v>
-      </c>
-      <c r="C36">
-        <v>34</v>
-      </c>
-      <c r="D36" t="s">
-        <v>122</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="F36" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="G36" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="H36" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I36" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="J36" s="2" t="str">
-        <f t="shared" ref="J36:J39" si="6">CONCATENATE("EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, ",B36,", ",C36,",'",D36,"','",E36,"','",F36,"',",G36,",'",H36,"',",I36,"; ")</f>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, 23, 34,'N/D','N/D','N/D',0,'N/D',0; </v>
-      </c>
-      <c r="M36" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B37" s="3">
-        <v>24</v>
-      </c>
-      <c r="C37">
-        <v>35</v>
-      </c>
-      <c r="D37" t="s">
-        <v>122</v>
-      </c>
-      <c r="E37" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="F37" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="G37" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="I37" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="J37" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, 24, 35,'N/D','NISSAN','2007',1.3,'3N6DD14547K040525',0; </v>
-      </c>
-      <c r="M37" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B38" s="3">
-        <v>25</v>
-      </c>
-      <c r="C38">
-        <v>36</v>
-      </c>
-      <c r="D38" t="s">
-        <v>122</v>
-      </c>
-      <c r="E38" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="F38" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="G38" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I38" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="J38" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, 25, 36,'N/D','N/D','N/D',0,'N/D',0; </v>
-      </c>
-      <c r="M38" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B39" s="3">
-        <v>26</v>
-      </c>
-      <c r="C39">
-        <v>37</v>
-      </c>
-      <c r="D39" t="s">
-        <v>122</v>
-      </c>
-      <c r="E39" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="F39" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="G39" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="H39" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="I39" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="J39" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, 26, 37,'N/D','NISSAN','2007',228.6,'3N6DD14568K002327',0; </v>
-      </c>
-      <c r="M39" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="2:13" hidden="1" x14ac:dyDescent="0.45">
-      <c r="B40" s="3">
-        <v>38</v>
-      </c>
-      <c r="C40">
-        <v>38</v>
-      </c>
-      <c r="D40" t="s">
-        <v>122</v>
-      </c>
-      <c r="E40" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="F40" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="G40" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I40" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="J40" s="2" t="e">
-        <f>CONCATENATE("EXECUTE [dbo].[PG_CI_DETALLE_PUNTO_VENTA] 0,0, ",B40,", ",C40,", ",#REF!,",",#REF!,",'",D40,"','",E40,"','",F40,"',",G40,",'",H40,"',",I40,",'",#REF!,"','",#REF!,"','",#REF!,"'; ")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M40" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B41" s="3">
-        <v>27</v>
-      </c>
-      <c r="C41">
-        <v>39</v>
-      </c>
-      <c r="D41" t="s">
-        <v>122</v>
-      </c>
-      <c r="E41" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="F41" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="G41" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I41" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="J41" s="2" t="str">
-        <f t="shared" ref="J41:J42" si="7">CONCATENATE("EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, ",B41,", ",C41,",'",D41,"','",E41,"','",F41,"',",G41,",'",H41,"',",I41,"; ")</f>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, 27, 39,'N/D','N/D','N/D',0,'N/D',0; </v>
-      </c>
-      <c r="M41" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B42" s="3">
-        <v>28</v>
-      </c>
-      <c r="C42">
-        <v>40</v>
-      </c>
-      <c r="D42" t="s">
-        <v>133</v>
-      </c>
-      <c r="E42" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="F42" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="G42" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I42" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="J42" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, 28, 40,'DV10353','N/D','N/D',0,'N/D',0; </v>
-      </c>
-      <c r="M42" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="2:13" hidden="1" x14ac:dyDescent="0.45">
-      <c r="B43" s="3">
-        <v>5</v>
-      </c>
-      <c r="C43">
-        <v>41</v>
-      </c>
-      <c r="D43" t="s">
-        <v>122</v>
-      </c>
-      <c r="E43" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="F43" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="G43" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="H43" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="I43" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="J43" s="2" t="e">
-        <f>CONCATENATE("EXECUTE [dbo].[PG_CI_DETALLE_AUTOTANQUE] 0,0, ",B43,", ",C43,", ",#REF!,",",#REF!,",'",D43,"','",E43,"','",F43,"',",G43,",'",H43,"',",I43,",'",#REF!,"','",#REF!,"','",#REF!,"'; ")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M43" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B44" s="3">
-        <v>29</v>
-      </c>
-      <c r="C44">
-        <v>42</v>
-      </c>
-      <c r="D44" t="s">
-        <v>134</v>
-      </c>
-      <c r="E44" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="F44" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="G44" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="H44" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I44" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="J44" s="2" t="str">
-        <f>CONCATENATE("EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, ",B44,", ",C44,",'",D44,"','",E44,"','",F44,"',",G44,",'",H44,"',",I44,"; ")</f>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, 29, 42,'DV10359','N/D','N/D',0,'N/D',0; </v>
-      </c>
-      <c r="M44" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="2:13" hidden="1" x14ac:dyDescent="0.45">
-      <c r="B45" s="3">
-        <v>43</v>
-      </c>
-      <c r="C45">
-        <v>43</v>
-      </c>
-      <c r="D45" t="s">
-        <v>122</v>
-      </c>
-      <c r="E45" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="F45" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="G45" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I45" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="J45" s="2" t="e">
-        <f>CONCATENATE("EXECUTE [dbo].[PG_CI_DETALLE_PUNTO_VENTA] 0,0, ",B45,", ",C45,", ",#REF!,",",#REF!,",'",D45,"','",E45,"','",F45,"',",G45,",'",H45,"',",I45,",'",#REF!,"','",#REF!,"','",#REF!,"'; ")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M45" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B46" s="3">
-        <v>30</v>
-      </c>
-      <c r="C46">
-        <v>44</v>
-      </c>
-      <c r="D46" t="s">
-        <v>122</v>
-      </c>
-      <c r="E46" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="F46" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="G46" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I46" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="J46" s="2" t="str">
-        <f t="shared" ref="J46:J49" si="8">CONCATENATE("EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, ",B46,", ",C46,",'",D46,"','",E46,"','",F46,"',",G46,",'",H46,"',",I46,"; ")</f>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, 30, 44,'N/D','CHEVROLET HEAVY DUTY','N/D',8911979,'N/D',0; </v>
-      </c>
-      <c r="M46" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B47" s="3">
-        <v>31</v>
-      </c>
-      <c r="C47">
-        <v>45</v>
-      </c>
-      <c r="D47" t="s">
-        <v>122</v>
-      </c>
-      <c r="E47" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="F47" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="G47" s="12">
-        <v>0</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I47" s="13" t="s">
-        <v>210</v>
-      </c>
-      <c r="J47" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, 31, 45,'N/D','N/D','N/D',0,'N/D',4750; </v>
-      </c>
-      <c r="M47" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B48" s="3">
-        <v>32</v>
-      </c>
-      <c r="C48">
-        <v>46</v>
-      </c>
-      <c r="D48" t="s">
-        <v>122</v>
-      </c>
-      <c r="E48" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="F48" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="G48" s="12">
-        <v>0</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I48" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="J48" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, 32, 46,'N/D','N/D','N/D',0,'N/D',3500; </v>
-      </c>
-      <c r="M48" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.45">
-      <c r="B49" s="3">
-        <v>33</v>
-      </c>
-      <c r="C49">
-        <v>47</v>
-      </c>
-      <c r="D49" t="s">
-        <v>122</v>
-      </c>
-      <c r="E49" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="F49" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="G49" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="I49" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="J49" s="2" t="str">
-        <f t="shared" si="8"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_DETALLE_PORTATIL] 0,0, 33, 47,'N/D','NISSAN VPM','2008',56309,'3NGDD14528K021599',1866; </v>
-      </c>
-      <c r="M49" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="2:13" hidden="1" x14ac:dyDescent="0.45">
-      <c r="B50" s="3">
-        <v>48</v>
-      </c>
-      <c r="C50">
-        <v>48</v>
-      </c>
-      <c r="D50" t="s">
-        <v>122</v>
-      </c>
-      <c r="E50" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="F50" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="G50" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I50" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="J50" s="2" t="e">
-        <f>CONCATENATE("EXECUTE [dbo].[PG_CI_DETALLE_PUNTO_VENTA] 0,0, ",B50,", ",C50,", ",#REF!,",",#REF!,",'",D50,"','",E50,"','",F50,"',",G50,",'",H50,"',",I50,",'",#REF!,"','",#REF!,"','",#REF!,"'; ")</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M50" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="2:13" hidden="1" x14ac:dyDescent="0.45">
-      <c r="B51" s="3">
-        <v>49</v>
-      </c>
-      <c r="C51">
-        <v>49</v>
-      </c>
-      <c r="D51" t="s">
-        <v>122</v>
-      </c>
-      <c r="E51" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="F51" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="G51" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I51" s="13" t="s">
-        <v>211</v>
-      </c>
-      <c r="J51" s="2" t="e">
-        <f>CONCATENATE("EXECUTE [dbo].[PG_CI_DETALLE_PUNTO_VENTA] 0,0, ",B51,", ",C51,", ",#REF!,",",#REF!,",'",D51,"','",E51,"','",F51,"',",G51,",'",H51,"',",I51,",'",#REF!,"','",#REF!,"','",#REF!,"'; ")</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="52" spans="2:13" hidden="1" x14ac:dyDescent="0.45">
-      <c r="B52" s="3">
-        <v>50</v>
-      </c>
-      <c r="C52">
-        <v>50</v>
-      </c>
-      <c r="D52" t="s">
-        <v>122</v>
-      </c>
-      <c r="E52" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="F52" s="12" t="s">
-        <v>122</v>
-      </c>
-      <c r="G52" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I52" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="J52" s="2" t="e">
-        <f>CONCATENATE("EXECUTE [dbo].[PG_CI_DETALLE_PUNTO_VENTA] 0,0, ",B52,", ",C52,", ",#REF!,",",#REF!,",'",D52,"','",E52,"','",F52,"',",G52,",'",H52,"',",I52,",'",#REF!,"','",#REF!,"','",#REF!,"'; ")</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="53" spans="2:13" hidden="1" x14ac:dyDescent="0.45">
-      <c r="I53" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="J53" s="2" t="e">
-        <f>CONCATENATE("EXECUTE [dbo].[PG_CI_DETALLE_PUNTO_VENTA] 0,0, ",B53,", ",C53,", ",#REF!,",",#REF!,",'",D53,"','",E53,"','",F53,"',",G53,",'",H53,"',",I53,",'",#REF!,"','",#REF!,"','",#REF!,"'; ")</f>
-        <v>#REF!</v>
+        <v>180</v>
+      </c>
+      <c r="J35" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 33, 47,3,'N/D','2008',56309,'3NGDD14528K021599',1866; </v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="M2:M53">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="3"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2787,9 +2010,9 @@
       <selection activeCell="I1" sqref="I1:I50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2839,7 +2062,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2889,7 +2112,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2939,7 +2162,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -2989,7 +2212,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -3039,7 +2262,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -3089,7 +2312,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -3139,7 +2362,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -3189,7 +2412,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -3239,7 +2462,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -3289,7 +2512,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -3339,7 +2562,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -3389,7 +2612,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -3439,7 +2662,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -3489,7 +2712,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -3539,7 +2762,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -3589,7 +2812,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -3639,7 +2862,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -3689,7 +2912,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -3739,7 +2962,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -3789,7 +3012,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -3839,7 +3062,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -3889,7 +3112,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -3939,7 +3162,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -3989,7 +3212,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -4039,7 +3262,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>1</v>
       </c>
@@ -4089,7 +3312,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -4139,7 +3362,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -4189,7 +3412,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -4239,7 +3462,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -4289,7 +3512,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>1</v>
       </c>
@@ -4339,7 +3562,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>1</v>
       </c>
@@ -4389,7 +3612,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>1</v>
       </c>
@@ -4439,7 +3662,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -4489,7 +3712,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>1</v>
       </c>
@@ -4539,7 +3762,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>1</v>
       </c>
@@ -4589,7 +3812,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>1</v>
       </c>
@@ -4639,7 +3862,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>1</v>
       </c>
@@ -4689,7 +3912,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>1</v>
       </c>
@@ -4739,7 +3962,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>1</v>
       </c>
@@ -4789,7 +4012,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>1</v>
       </c>
@@ -4839,7 +4062,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>1</v>
       </c>
@@ -4889,7 +4112,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>1</v>
       </c>
@@ -4939,7 +4162,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>1</v>
       </c>
@@ -4989,7 +4212,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>1</v>
       </c>
@@ -5039,7 +4262,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>1</v>
       </c>
@@ -5089,7 +4312,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>1</v>
       </c>
@@ -5139,7 +4362,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>1</v>
       </c>
@@ -5189,7 +4412,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>1</v>
       </c>
@@ -5239,7 +4462,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Ultimos ajustes del Jueves
</commit_message>
<xml_diff>
--- a/Scripts_R210_FuerzaVenta/LIQ19_R110_30.b_CI_Ficha_Portatil_20190131_JAR.XLSX
+++ b/Scripts_R210_FuerzaVenta/LIQ19_R110_30.b_CI_Ficha_Portatil_20190131_JAR.XLSX
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tomza.TI\JArciniegaR.TI\1.SOL_Soluciones\LIQ19_Liquidaciones\Codigo\CodigoSQL\LIQ19_Liberacion_R0.00_Base_V0004\Scripts_R210_FuerzaVenta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tomza.TI\JArciniegaR.TI\1.SOL_Soluciones\LIQ19_Liquidaciones\Codigo\CodigoSQL\LIQ19_Liberacion_R0.00_Base_V0006\Scripts_R210_FuerzaVenta\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -952,10 +952,10 @@
   <dimension ref="B2:Q35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G42" sqref="G42"/>
+      <selection pane="bottomRight" activeCell="J3" sqref="J3:J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1011,7 +1011,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="12">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="E3" t="s">
         <v>111</v>
@@ -1030,7 +1030,7 @@
       </c>
       <c r="J3" s="2" t="str">
         <f>CONCATENATE("EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, ",B3,", ",C3,",",D3,",'",E3,"','",F3,"',",G3,",'",H3,"',",I3,"; ")</f>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 1, 2,1,'BCD345','2006',233859,'3GBKC34G55M118806',5000; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 1, 2,101,'BCD345','2006',233859,'3GBKC34G55M118806',5000; </v>
       </c>
       <c r="N3" s="6"/>
     </row>
@@ -1042,7 +1042,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="12">
-        <v>2</v>
+        <v>102</v>
       </c>
       <c r="E4" t="s">
         <v>112</v>
@@ -1061,7 +1061,7 @@
       </c>
       <c r="J4" s="2" t="str">
         <f t="shared" ref="J4:J35" si="0">CONCATENATE("EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, ",B4,", ",C4,",",D4,",'",E4,"','",F4,"',",G4,",'",H4,"',",I4,"; ")</f>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 2, 4,2,'FEFE889','2002',1522039,'1GDJ7H1E4J901664',11315; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 2, 4,102,'FEFE889','2002',1522039,'1GDJ7H1E4J901664',11315; </v>
       </c>
       <c r="N4" s="7"/>
     </row>
@@ -1073,7 +1073,7 @@
         <v>5</v>
       </c>
       <c r="D5" s="12">
-        <v>3</v>
+        <v>103</v>
       </c>
       <c r="E5" t="s">
         <v>113</v>
@@ -1092,7 +1092,7 @@
       </c>
       <c r="J5" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 3, 5,3,'MAT123','2005',0,'3GBKC34GX5M101984',5000; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 3, 5,103,'MAT123','2005',0,'3GBKC34GX5M101984',5000; </v>
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
@@ -1103,7 +1103,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="12">
-        <v>4</v>
+        <v>104</v>
       </c>
       <c r="E6" t="s">
         <v>118</v>
@@ -1122,7 +1122,7 @@
       </c>
       <c r="J6" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 4, 6,4,'N/D','2006',164292,'3GBKC34G55M118837',4300; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 4, 6,104,'N/D','2006',164292,'3GBKC34G55M118837',4300; </v>
       </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
@@ -1133,7 +1133,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="12">
-        <v>5</v>
+        <v>105</v>
       </c>
       <c r="E7" t="s">
         <v>119</v>
@@ -1152,7 +1152,7 @@
       </c>
       <c r="J7" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 5, 7,5,'DV10365','2006',141076,'3GBKC34GX5M118915',5000; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 5, 7,105,'DV10365','2006',141076,'3GBKC34GX5M118915',5000; </v>
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.25">
@@ -1163,7 +1163,7 @@
         <v>9</v>
       </c>
       <c r="D8" s="12">
-        <v>6</v>
+        <v>106</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>120</v>
@@ -1182,7 +1182,7 @@
       </c>
       <c r="J8" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 6, 9,6,'ZTV6503','1997',1578795,'1GDG6H1P9RJ519414',12500; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 6, 9,106,'ZTV6503','1997',1578795,'1GDG6H1P9RJ519414',12500; </v>
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
@@ -1193,7 +1193,7 @@
         <v>10</v>
       </c>
       <c r="D9" s="12">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="E9" t="s">
         <v>121</v>
@@ -1212,7 +1212,7 @@
       </c>
       <c r="J9" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 7, 10,1,'DW31616','N/D',0,'N/D',12500; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 7, 10,101,'DW31616','N/D',0,'N/D',12500; </v>
       </c>
       <c r="N9" s="15"/>
     </row>
@@ -1224,7 +1224,7 @@
         <v>12</v>
       </c>
       <c r="D10" s="12">
-        <v>2</v>
+        <v>102</v>
       </c>
       <c r="E10" t="s">
         <v>122</v>
@@ -1243,7 +1243,7 @@
       </c>
       <c r="J10" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 8, 12,2,'DV10363','1990',61784,'1GBM7H1P2PJ101461',12500; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 8, 12,102,'DV10363','1990',61784,'1GBM7H1P2PJ101461',12500; </v>
       </c>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
@@ -1254,7 +1254,7 @@
         <v>14</v>
       </c>
       <c r="D11" s="12">
-        <v>3</v>
+        <v>103</v>
       </c>
       <c r="E11" t="s">
         <v>118</v>
@@ -1273,7 +1273,7 @@
       </c>
       <c r="J11" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 9, 14,3,'N/D','2005',0,'3GBJ6H1E45M105516',8250; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 9, 14,103,'N/D','2005',0,'3GBJ6H1E45M105516',8250; </v>
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
@@ -1284,7 +1284,7 @@
         <v>15</v>
       </c>
       <c r="D12" s="12">
-        <v>4</v>
+        <v>104</v>
       </c>
       <c r="E12" t="s">
         <v>118</v>
@@ -1303,7 +1303,7 @@
       </c>
       <c r="J12" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 10, 15,4,'N/D','1995',2099804,'1G017H1P45J520018',12500; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 10, 15,104,'N/D','1995',2099804,'1G017H1P45J520018',12500; </v>
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.25">
@@ -1314,7 +1314,7 @@
         <v>16</v>
       </c>
       <c r="D13" s="12">
-        <v>5</v>
+        <v>105</v>
       </c>
       <c r="E13" t="s">
         <v>123</v>
@@ -1333,7 +1333,7 @@
       </c>
       <c r="J13" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 11, 16,5,'DV10362','1992',1881350,'1GDG6H1T7PJ504326',8670; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 11, 16,105,'DV10362','1992',1881350,'1GDG6H1T7PJ504326',8670; </v>
       </c>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
@@ -1344,7 +1344,7 @@
         <v>17</v>
       </c>
       <c r="D14" s="12">
-        <v>6</v>
+        <v>106</v>
       </c>
       <c r="E14" t="s">
         <v>118</v>
@@ -1363,7 +1363,7 @@
       </c>
       <c r="J14" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 12, 17,6,'N/D','2002',2443861,'3GBM7H1E62M104342',12500; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 12, 17,106,'N/D','2002',2443861,'3GBM7H1E62M104342',12500; </v>
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
@@ -1374,7 +1374,7 @@
         <v>19</v>
       </c>
       <c r="D15" s="12">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="E15" t="s">
         <v>124</v>
@@ -1393,7 +1393,7 @@
       </c>
       <c r="J15" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 13, 19,1,'DY-2983','N/D',0,'N/D',12500; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 13, 19,101,'DY-2983','N/D',0,'N/D',12500; </v>
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
@@ -1404,7 +1404,7 @@
         <v>20</v>
       </c>
       <c r="D16" s="12">
-        <v>2</v>
+        <v>102</v>
       </c>
       <c r="E16" t="s">
         <v>118</v>
@@ -1423,7 +1423,7 @@
       </c>
       <c r="J16" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 14, 20,2,'N/D','N/D',0,'N/D',12500; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 14, 20,102,'N/D','N/D',0,'N/D',12500; </v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
@@ -1434,7 +1434,7 @@
         <v>22</v>
       </c>
       <c r="D17" s="12">
-        <v>3</v>
+        <v>103</v>
       </c>
       <c r="E17" t="s">
         <v>125</v>
@@ -1453,7 +1453,7 @@
       </c>
       <c r="J17" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 15, 22,3,'DV10456','1995',1276028,'1GDG6H1P6TJ504599',12500; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 15, 22,103,'DV10456','1995',1276028,'1GDG6H1P6TJ504599',12500; </v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
@@ -1464,7 +1464,7 @@
         <v>24</v>
       </c>
       <c r="D18" s="12">
-        <v>4</v>
+        <v>104</v>
       </c>
       <c r="E18" t="s">
         <v>118</v>
@@ -1483,7 +1483,7 @@
       </c>
       <c r="J18" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 16, 24,4,'N/D','N/D',0,'N/D',6850; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 16, 24,104,'N/D','N/D',0,'N/D',6850; </v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
@@ -1494,7 +1494,7 @@
         <v>25</v>
       </c>
       <c r="D19" s="12">
-        <v>5</v>
+        <v>105</v>
       </c>
       <c r="E19" t="s">
         <v>118</v>
@@ -1513,7 +1513,7 @@
       </c>
       <c r="J19" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 17, 25,5,'N/D','2010',29056,'013FB0473C4F544B',0; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 17, 25,105,'N/D','2010',29056,'013FB0473C4F544B',0; </v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
@@ -1524,7 +1524,7 @@
         <v>26</v>
       </c>
       <c r="D20" s="12">
-        <v>6</v>
+        <v>106</v>
       </c>
       <c r="E20" t="s">
         <v>118</v>
@@ -1543,7 +1543,7 @@
       </c>
       <c r="J20" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 18, 26,6,'N/D','2010',17711,'0136B07390508612',0; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 18, 26,106,'N/D','2010',17711,'0136B07390508612',0; </v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
@@ -1554,7 +1554,7 @@
         <v>27</v>
       </c>
       <c r="D21" s="12">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="E21" t="s">
         <v>126</v>
@@ -1573,7 +1573,7 @@
       </c>
       <c r="J21" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 19, 27,1,'DV10419','N/D',0,'N/D',0; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 19, 27,101,'DV10419','N/D',0,'N/D',0; </v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
@@ -1584,7 +1584,7 @@
         <v>29</v>
       </c>
       <c r="D22" s="12">
-        <v>2</v>
+        <v>102</v>
       </c>
       <c r="E22" t="s">
         <v>118</v>
@@ -1603,7 +1603,7 @@
       </c>
       <c r="J22" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 20, 29,2,'N/D','2010',0,'0136B07390508612',0; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 20, 29,102,'N/D','2010',0,'0136B07390508612',0; </v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
@@ -1614,7 +1614,7 @@
         <v>30</v>
       </c>
       <c r="D23" s="12">
-        <v>3</v>
+        <v>103</v>
       </c>
       <c r="E23" t="s">
         <v>118</v>
@@ -1633,7 +1633,7 @@
       </c>
       <c r="J23" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 21, 30,3,'N/D','2010',22098,'013AB067801076420',0; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 21, 30,103,'N/D','2010',22098,'013AB067801076420',0; </v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
@@ -1644,7 +1644,7 @@
         <v>32</v>
       </c>
       <c r="D24" s="12">
-        <v>4</v>
+        <v>104</v>
       </c>
       <c r="E24" t="s">
         <v>118</v>
@@ -1663,7 +1663,7 @@
       </c>
       <c r="J24" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 22, 32,4,'N/D','N/D',0,'N/D',0; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 22, 32,104,'N/D','N/D',0,'N/D',0; </v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
@@ -1674,7 +1674,7 @@
         <v>34</v>
       </c>
       <c r="D25" s="12">
-        <v>5</v>
+        <v>105</v>
       </c>
       <c r="E25" t="s">
         <v>118</v>
@@ -1693,7 +1693,7 @@
       </c>
       <c r="J25" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 23, 34,5,'N/D','N/D',0,'N/D',0; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 23, 34,105,'N/D','N/D',0,'N/D',0; </v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
@@ -1704,7 +1704,7 @@
         <v>35</v>
       </c>
       <c r="D26" s="12">
-        <v>6</v>
+        <v>106</v>
       </c>
       <c r="E26" t="s">
         <v>118</v>
@@ -1723,7 +1723,7 @@
       </c>
       <c r="J26" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 24, 35,6,'N/D','2007',1.3,'3N6DD14547K040525',0; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 24, 35,106,'N/D','2007',1.3,'3N6DD14547K040525',0; </v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
@@ -1734,7 +1734,7 @@
         <v>36</v>
       </c>
       <c r="D27" s="12">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="E27" t="s">
         <v>118</v>
@@ -1753,7 +1753,7 @@
       </c>
       <c r="J27" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 25, 36,1,'N/D','N/D',0,'N/D',0; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 25, 36,101,'N/D','N/D',0,'N/D',0; </v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
@@ -1764,7 +1764,7 @@
         <v>37</v>
       </c>
       <c r="D28" s="12">
-        <v>2</v>
+        <v>102</v>
       </c>
       <c r="E28" t="s">
         <v>118</v>
@@ -1783,7 +1783,7 @@
       </c>
       <c r="J28" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 26, 37,2,'N/D','2007',228.6,'3N6DD14568K002327',0; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 26, 37,102,'N/D','2007',228.6,'3N6DD14568K002327',0; </v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
@@ -1794,7 +1794,7 @@
         <v>39</v>
       </c>
       <c r="D29" s="12">
-        <v>3</v>
+        <v>103</v>
       </c>
       <c r="E29" t="s">
         <v>118</v>
@@ -1813,7 +1813,7 @@
       </c>
       <c r="J29" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 27, 39,3,'N/D','N/D',0,'N/D',0; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 27, 39,103,'N/D','N/D',0,'N/D',0; </v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
@@ -1824,7 +1824,7 @@
         <v>40</v>
       </c>
       <c r="D30" s="12">
-        <v>4</v>
+        <v>104</v>
       </c>
       <c r="E30" t="s">
         <v>127</v>
@@ -1843,7 +1843,7 @@
       </c>
       <c r="J30" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 28, 40,4,'DV10353','N/D',0,'N/D',0; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 28, 40,104,'DV10353','N/D',0,'N/D',0; </v>
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
@@ -1854,7 +1854,7 @@
         <v>42</v>
       </c>
       <c r="D31" s="12">
-        <v>5</v>
+        <v>105</v>
       </c>
       <c r="E31" t="s">
         <v>128</v>
@@ -1873,7 +1873,7 @@
       </c>
       <c r="J31" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 29, 42,5,'DV10359','N/D',0,'N/D',0; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 29, 42,105,'DV10359','N/D',0,'N/D',0; </v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
@@ -1884,7 +1884,7 @@
         <v>44</v>
       </c>
       <c r="D32" s="12">
-        <v>6</v>
+        <v>106</v>
       </c>
       <c r="E32" t="s">
         <v>118</v>
@@ -1903,7 +1903,7 @@
       </c>
       <c r="J32" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 30, 44,6,'N/D','N/D',8911979,'N/D',0; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 30, 44,106,'N/D','N/D',8911979,'N/D',0; </v>
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
@@ -1914,7 +1914,7 @@
         <v>45</v>
       </c>
       <c r="D33" s="12">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="E33" t="s">
         <v>118</v>
@@ -1933,7 +1933,7 @@
       </c>
       <c r="J33" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 31, 45,1,'N/D','N/D',0,'N/D',4750; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 31, 45,101,'N/D','N/D',0,'N/D',4750; </v>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
@@ -1944,7 +1944,7 @@
         <v>46</v>
       </c>
       <c r="D34" s="12">
-        <v>2</v>
+        <v>102</v>
       </c>
       <c r="E34" t="s">
         <v>118</v>
@@ -1963,7 +1963,7 @@
       </c>
       <c r="J34" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 32, 46,2,'N/D','N/D',0,'N/D',3500; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 32, 46,102,'N/D','N/D',0,'N/D',3500; </v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
@@ -1974,7 +1974,7 @@
         <v>47</v>
       </c>
       <c r="D35" s="12">
-        <v>3</v>
+        <v>103</v>
       </c>
       <c r="E35" t="s">
         <v>118</v>
@@ -1993,7 +1993,7 @@
       </c>
       <c r="J35" s="2" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 33, 47,3,'N/D','2008',56309,'3NGDD14528K021599',1866; </v>
+        <v xml:space="preserve">EXECUTE [dbo].[PG_CI_FICHA_PORTATIL] 0,0, 33, 47,103,'N/D','2008',56309,'3NGDD14528K021599',1866; </v>
       </c>
     </row>
   </sheetData>

</xml_diff>